<commit_message>
updated ph207, ep1 and f7
</commit_message>
<xml_diff>
--- a/nf/genomes.xlsx
+++ b/nf/genomes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Library/Containers/com.panic.transmit.mas/Data/Library/Caches/Transmit/5C99CA29-BCAF-4F64-8AFC-A95DEE9CDB88/login.msi.umn.edu/panfs/roc/groups/15/springer/zhoux379/projects/genome/nf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Library/Containers/com.panic.transmit.mas/Data/Library/Caches/Transmit/B94C5795-954D-4CD3-A4A1-142A238C3D35/login.msi.umn.edu/panfs/roc/groups/15/springer/zhoux379/projects/genome/nf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8A4515-4033-084B-9906-192FED15D279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E78FA9-FFB6-DE44-AE96-2FACEDC815AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5340" yWindow="3140" windowWidth="21960" windowHeight="17860" xr2:uid="{80E7688E-3C92-F248-929C-B53449277935}"/>
   </bookViews>
@@ -1814,10 +1814,10 @@
   <dimension ref="A1:Z102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D67" sqref="D67"/>
+      <selection pane="bottomRight" activeCell="L94" sqref="L94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5464,7 +5464,7 @@
       </c>
       <c r="K71" s="1"/>
       <c r="L71" s="2">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="M71" s="1" t="s">
         <v>54</v>
@@ -6869,7 +6869,7 @@
       </c>
       <c r="K97" s="1"/>
       <c r="L97" s="1">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="M97" s="1" t="s">
         <v>7</v>
@@ -6977,7 +6977,7 @@
       </c>
       <c r="K99" s="1"/>
       <c r="L99" s="1">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="M99" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
updated Taz source to gzipped version
</commit_message>
<xml_diff>
--- a/nf/genomes.xlsx
+++ b/nf/genomes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Library/Containers/com.panic.transmit.mas/Data/Library/Caches/Transmit/C5DDA3E0-626E-435C-984B-AD2EA0E8703C/192.168.1.19/datalus/weiyu/projects/genome/nf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Library/Containers/com.panic.transmit.mas/Data/Library/Caches/Transmit/486C5284-E143-42A1-9BC3-A5523549CBD3/192.168.1.19/datalus/weiyu/projects/genome/nf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70C81B3-9572-3141-BF03-9440BDE211E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2FD1AD-F9DC-8847-B8C0-FB6C751B09DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2360" yWindow="3280" windowWidth="21960" windowHeight="17860" xr2:uid="{80E7688E-3C92-F248-929C-B53449277935}"/>
   </bookViews>
@@ -1146,9 +1146,6 @@
     <t>raw_Atauschii/Atauschii_AY17/AY17.all_gene.gff</t>
   </si>
   <si>
-    <t>raw_Atauschii/raw_AS60/AS60.final.fasta</t>
-  </si>
-  <si>
     <t>B73 RefGen_v5</t>
   </si>
   <si>
@@ -1269,9 +1266,6 @@
     <t>B73v4</t>
   </si>
   <si>
-    <t>raw_Atauschii/raw_AS60/final.as60.gene.gff3</t>
-  </si>
-  <si>
     <t>Taestivum_z</t>
   </si>
   <si>
@@ -1281,10 +1275,16 @@
     <t>Taz</t>
   </si>
   <si>
-    <t>raw_Atauschii/raw_AS60/combine_Ta_genome.fa</t>
-  </si>
-  <si>
-    <t>raw_Atauschii/raw_AS60/combine_Ta_genome.gff3</t>
+    <t>raw_Atauschii/raw_AS60/combine_Ta_genome.fa.gz</t>
+  </si>
+  <si>
+    <t>raw_Atauschii/raw_AS60/combine_Ta_genome.gff3.gz</t>
+  </si>
+  <si>
+    <t>raw_Atauschii/raw_AS60/AS60.final.fasta.gz</t>
+  </si>
+  <si>
+    <t>raw_Atauschii/raw_AS60/final.as60.gene.gff3.gz</t>
   </si>
 </sst>
 </file>
@@ -1856,7 +1856,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X29" sqref="X29"/>
+      <selection pane="bottomRight" activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3858,16 +3858,16 @@
     </row>
     <row r="39" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B39" t="s">
         <v>324</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>6</v>
@@ -3875,10 +3875,10 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>159</v>
@@ -4250,10 +4250,10 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1" t="s">
-        <v>370</v>
+        <v>415</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>159</v>
@@ -4313,10 +4313,10 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>373</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>159</v>
@@ -4371,10 +4371,10 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>375</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>159</v>
@@ -4419,10 +4419,10 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="I50" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>159</v>
@@ -4467,10 +4467,10 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="I51" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>379</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>159</v>
@@ -4515,10 +4515,10 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>381</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>159</v>
@@ -4563,10 +4563,10 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>383</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>159</v>
@@ -4611,10 +4611,10 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="I54" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>385</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>159</v>
@@ -4659,10 +4659,10 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>386</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>387</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>159</v>
@@ -4707,10 +4707,10 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="I56" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>389</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>159</v>
@@ -4755,10 +4755,10 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="I57" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>391</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>159</v>
@@ -4803,10 +4803,10 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="I58" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>393</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>159</v>
@@ -4851,10 +4851,10 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="I59" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>395</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>159</v>
@@ -4907,10 +4907,10 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="I60" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>159</v>
@@ -4955,10 +4955,10 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="I61" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>399</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>159</v>
@@ -5003,10 +5003,10 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="I62" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>401</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>159</v>
@@ -5051,10 +5051,10 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="I63" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>403</v>
       </c>
       <c r="J63" s="1" t="s">
         <v>159</v>
@@ -5107,10 +5107,10 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="I64" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>405</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>159</v>
@@ -5155,10 +5155,10 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="I65" s="1" t="s">
         <v>406</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>407</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>159</v>
@@ -5203,10 +5203,10 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>409</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>159</v>
@@ -5307,7 +5307,7 @@
         <v>68</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>66</v>
@@ -5379,7 +5379,7 @@
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H69" s="4" t="s">
         <v>52</v>

</xml_diff>